<commit_message>
updated ExcelFileReader in DataProviders Class
</commit_message>
<xml_diff>
--- a/Resources/excelFiles/sheet35.xlsx
+++ b/Resources/excelFiles/sheet35.xlsx
@@ -439,19 +439,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="2"/>
   <cols>
     <col min="2" max="2" width="9.375"/>
     <col min="4" max="4" width="11.125"/>
+    <col min="6" max="6" width="9.375"/>
+    <col min="8" max="8" width="11.125"/>
+    <col min="10" max="10" width="9.375"/>
+    <col min="12" max="12" width="11.125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +468,32 @@
       <c r="D1" s="1">
         <v>498723.45</v>
       </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="1">
+        <v>498723.45</v>
+      </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1">
+        <v>498723.45</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:12">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -478,8 +506,32 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
+      <c r="E2" s="2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -490,6 +542,30 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>98654321</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>98654321</v>
+      </c>
+      <c r="K3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>